<commit_message>
Set up Naked Functions manual outline
</commit_message>
<xml_diff>
--- a/Documentation/Naked Functions/Naked Functions - Attributes.xlsx
+++ b/Documentation/Naked Functions/Naked Functions - Attributes.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24315"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\NakedObjectsFramework\Documentation\Naked Functions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93C0C969-DDE4-42CB-8A93-019D46ED72D6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB00A8BD-D201-4019-8CC0-8E565B4DD3B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1305" yWindow="-15870" windowWidth="25440" windowHeight="15390" xr2:uid="{F90638A0-5B97-415D-B8E6-E7D5161399E3}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="58">
   <si>
     <t>[Bounded]</t>
   </si>
@@ -249,6 +249,12 @@
   </si>
   <si>
     <t>Specifies that a string parameter should be rendered as a multi-line text field, with specified number of lines,  scrollable.  The Width property is unused by the current client, but is exposed on the Resftul API for custom use.</t>
+  </si>
+  <si>
+    <t>[Disabled]</t>
+  </si>
+  <si>
+    <t>Renders parameter, but does not permit the user to change that value (useful as an advisory).</t>
   </si>
 </sst>
 </file>
@@ -373,7 +379,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -396,9 +402,27 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
@@ -407,23 +431,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -739,10 +754,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19D1B0AD-A80F-47A6-B71C-21BAE0653708}">
-  <dimension ref="A1:E24"/>
+  <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10:E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -776,8 +791,8 @@
         <v>28</v>
       </c>
       <c r="C2" s="11"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="13"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="12"/>
     </row>
     <row r="3" spans="1:5" ht="58" x14ac:dyDescent="0.35">
       <c r="A3" s="8" t="s">
@@ -795,8 +810,8 @@
         <v>2</v>
       </c>
       <c r="B4" s="11"/>
-      <c r="C4" s="12"/>
-      <c r="D4" s="13"/>
+      <c r="C4" s="16"/>
+      <c r="D4" s="12"/>
       <c r="E4" s="4" t="s">
         <v>30</v>
       </c>
@@ -805,253 +820,264 @@
       <c r="A5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="20" t="s">
+      <c r="B5" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="C5" s="21"/>
-      <c r="D5" s="21"/>
-      <c r="E5" s="22"/>
-    </row>
-    <row r="6" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="C5" s="14"/>
+      <c r="D5" s="14"/>
+      <c r="E5" s="15"/>
+    </row>
+    <row r="6" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A6" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="B6" s="23"/>
+      <c r="C6" s="24"/>
+      <c r="D6" s="24"/>
+      <c r="E6" s="25" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A7" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="11"/>
-      <c r="C6" s="13"/>
-      <c r="D6" s="4" t="s">
+      <c r="B7" s="11"/>
+      <c r="C7" s="12"/>
+      <c r="D7" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="E6" s="3"/>
-    </row>
-    <row r="7" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A7" s="8" t="s">
+      <c r="E7" s="3"/>
+    </row>
+    <row r="8" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A8" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="11"/>
-      <c r="C7" s="13"/>
-      <c r="D7" s="4" t="s">
+      <c r="B8" s="11"/>
+      <c r="C8" s="12"/>
+      <c r="D8" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="E7" s="3"/>
-    </row>
-    <row r="8" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A8" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" s="3"/>
-      <c r="C8" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="D8" s="11"/>
-      <c r="E8" s="13"/>
+      <c r="E8" s="3"/>
     </row>
     <row r="9" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A9" s="8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B9" s="3"/>
       <c r="C9" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D9" s="11"/>
-      <c r="E9" s="13"/>
+      <c r="E9" s="12"/>
     </row>
     <row r="10" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A10" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="3"/>
+      <c r="C10" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D10" s="11"/>
+      <c r="E10" s="12"/>
+    </row>
+    <row r="11" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A11" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="11"/>
-      <c r="C10" s="12"/>
-      <c r="D10" s="13"/>
-      <c r="E10" s="4" t="s">
+      <c r="B11" s="11"/>
+      <c r="C11" s="16"/>
+      <c r="D11" s="12"/>
+      <c r="E11" s="4" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="87" x14ac:dyDescent="0.35">
-      <c r="A11" s="8" t="s">
+    <row r="12" spans="1:5" ht="87" x14ac:dyDescent="0.35">
+      <c r="A12" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="6"/>
-      <c r="C11" s="4" t="s">
+      <c r="B12" s="6"/>
+      <c r="C12" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="D11" s="4" t="s">
+      <c r="D12" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="E11" s="7"/>
-    </row>
-    <row r="12" spans="1:5" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A12" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="B12" s="11"/>
-      <c r="C12" s="12"/>
-      <c r="D12" s="13"/>
-      <c r="E12" s="4" t="s">
-        <v>38</v>
-      </c>
+      <c r="E12" s="7"/>
     </row>
     <row r="13" spans="1:5" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A13" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B13" s="11"/>
+      <c r="C13" s="16"/>
+      <c r="D13" s="12"/>
+      <c r="E13" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A14" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="3"/>
-      <c r="C13" s="4" t="s">
+      <c r="B14" s="3"/>
+      <c r="C14" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="D13" s="10" t="s">
+      <c r="D14" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="E13" s="4" t="s">
+      <c r="E14" s="4" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A14" s="8" t="s">
+    <row r="15" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A15" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="17" t="s">
+      <c r="B15" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="C14" s="18"/>
-      <c r="D14" s="18"/>
-      <c r="E14" s="19"/>
-    </row>
-    <row r="15" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A15" s="8" t="s">
+      <c r="C15" s="18"/>
+      <c r="D15" s="18"/>
+      <c r="E15" s="19"/>
+    </row>
+    <row r="16" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A16" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="11"/>
-      <c r="C15" s="12"/>
-      <c r="D15" s="13"/>
-      <c r="E15" s="4" t="s">
+      <c r="B16" s="11"/>
+      <c r="C16" s="16"/>
+      <c r="D16" s="12"/>
+      <c r="E16" s="4" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A16" s="8" t="s">
+    <row r="17" spans="1:5" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A17" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="B16" s="11"/>
-      <c r="C16" s="13"/>
-      <c r="D16" s="4" t="s">
+      <c r="B17" s="11"/>
+      <c r="C17" s="12"/>
+      <c r="D17" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="E16" s="3"/>
-    </row>
-    <row r="17" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A17" s="9" t="s">
+      <c r="E17" s="3"/>
+    </row>
+    <row r="18" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A18" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="B17" s="4" t="s">
+      <c r="B18" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="C17" s="11"/>
-      <c r="D17" s="12"/>
-      <c r="E17" s="13"/>
-    </row>
-    <row r="18" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A18" s="9" t="s">
+      <c r="C18" s="11"/>
+      <c r="D18" s="16"/>
+      <c r="E18" s="12"/>
+    </row>
+    <row r="19" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A19" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="B18" s="14" t="s">
+      <c r="B19" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="C18" s="15"/>
-      <c r="D18" s="15"/>
-      <c r="E18" s="16"/>
-    </row>
-    <row r="19" spans="1:5" ht="58" x14ac:dyDescent="0.35">
-      <c r="A19" s="9" t="s">
+      <c r="C19" s="21"/>
+      <c r="D19" s="21"/>
+      <c r="E19" s="22"/>
+    </row>
+    <row r="20" spans="1:5" ht="58" x14ac:dyDescent="0.35">
+      <c r="A20" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="B19" s="11"/>
-      <c r="C19" s="12"/>
-      <c r="D19" s="13"/>
-      <c r="E19" s="4" t="s">
+      <c r="B20" s="11"/>
+      <c r="C20" s="16"/>
+      <c r="D20" s="12"/>
+      <c r="E20" s="4" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A20" s="9" t="s">
+    <row r="21" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A21" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="B20" s="5" t="s">
+      <c r="B21" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="C20" s="4" t="s">
+      <c r="C21" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="D20" s="4" t="s">
+      <c r="D21" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="E20" s="7"/>
-    </row>
-    <row r="21" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A21" s="9" t="s">
+      <c r="E21" s="7"/>
+    </row>
+    <row r="22" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A22" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="B21" s="3"/>
-      <c r="C21" s="14" t="s">
+      <c r="B22" s="3"/>
+      <c r="C22" s="20" t="s">
         <v>50</v>
       </c>
-      <c r="D21" s="16"/>
-      <c r="E21" s="3"/>
-    </row>
-    <row r="22" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A22" s="9" t="s">
+      <c r="D22" s="22"/>
+      <c r="E22" s="3"/>
+    </row>
+    <row r="23" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A23" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="B22" s="11"/>
-      <c r="C22" s="12"/>
-      <c r="D22" s="13"/>
-      <c r="E22" s="4" t="s">
+      <c r="B23" s="11"/>
+      <c r="C23" s="16"/>
+      <c r="D23" s="12"/>
+      <c r="E23" s="4" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="159.5" x14ac:dyDescent="0.35">
-      <c r="A23" s="9" t="s">
+    <row r="24" spans="1:5" ht="159.5" x14ac:dyDescent="0.35">
+      <c r="A24" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="B23" s="3"/>
-      <c r="C23" s="4" t="s">
+      <c r="B24" s="3"/>
+      <c r="C24" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="D23" s="11"/>
-      <c r="E23" s="13"/>
-    </row>
-    <row r="24" spans="1:5" ht="87" x14ac:dyDescent="0.35">
-      <c r="A24" s="9" t="s">
+      <c r="D24" s="11"/>
+      <c r="E24" s="12"/>
+    </row>
+    <row r="25" spans="1:5" ht="87" x14ac:dyDescent="0.35">
+      <c r="A25" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="B24" s="4" t="s">
+      <c r="B25" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="C24" s="11"/>
-      <c r="D24" s="12"/>
-      <c r="E24" s="13"/>
+      <c r="C25" s="11"/>
+      <c r="D25" s="16"/>
+      <c r="E25" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="C25:E25"/>
+    <mergeCell ref="C18:E18"/>
+    <mergeCell ref="B19:E19"/>
+    <mergeCell ref="B20:D20"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="B23:D23"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="B11:D11"/>
+    <mergeCell ref="B13:D13"/>
+    <mergeCell ref="B15:E15"/>
+    <mergeCell ref="B16:D16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="D10:E10"/>
     <mergeCell ref="D9:E9"/>
-    <mergeCell ref="D8:E8"/>
     <mergeCell ref="B5:E5"/>
     <mergeCell ref="C2:E2"/>
     <mergeCell ref="B4:D4"/>
-    <mergeCell ref="B6:C6"/>
     <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B10:D10"/>
-    <mergeCell ref="B12:D12"/>
-    <mergeCell ref="B14:E14"/>
-    <mergeCell ref="B15:D15"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="C24:E24"/>
-    <mergeCell ref="C17:E17"/>
-    <mergeCell ref="B18:E18"/>
-    <mergeCell ref="B19:D19"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="B22:D22"/>
-    <mergeCell ref="D23:E23"/>
+    <mergeCell ref="B8:C8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>